<commit_message>
DataBoard UI 간략하게 구성
</commit_message>
<xml_diff>
--- a/Assets/Data/Excels/Animal.xlsx
+++ b/Assets/Data/Excels/Animal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataGenerator\Assets\Data\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataGenerator\Assets\Data\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C44775-CD63-4C05-BF48-CB7BA85079E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8FC3EE-2DC1-4794-A918-2A13B18BEE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,10 @@
   </si>
   <si>
     <t>ANIMAL_NINA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANIMAL_LALI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -506,6 +510,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>